<commit_message>
mise à jour du micro service
ajout d'un nouveau champs dans le fichier json et modifier de la template excel
</commit_message>
<xml_diff>
--- a/PrintExcelToPdf/Templates/template_sunu.xlsx
+++ b/PrintExcelToPdf/Templates/template_sunu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gedeo\source\repos\PrintExcelToPdf\PrintExcelToPdf\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5795662-B139-4E2E-A22C-AF29EBA7AFF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660A3D7B-BFA2-4687-838D-7801C0FD70B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BDB7740D-B914-44FE-88FD-0981D9AB0366}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>15/03/2025</t>
+    <t>AS1</t>
   </si>
 </sst>
 </file>
@@ -46,7 +46,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +61,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -70,7 +77,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -78,14 +85,34 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="dotted">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -308,6 +335,13 @@
             <a:schemeClr val="tx1"/>
           </a:solidFill>
         </a:ln>
+        <a:scene3d>
+          <a:camera prst="orthographicFront"/>
+          <a:lightRig rig="threePt" dir="t"/>
+        </a:scene3d>
+        <a:sp3d>
+          <a:bevelT w="101600" prst="riblet"/>
+        </a:sp3d>
       </xdr:spPr>
       <xdr:style>
         <a:lnRef idx="2">
@@ -330,7 +364,19 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr algn="l"/>
-          <a:endParaRPr lang="LID4096" sz="1100"/>
+          <a:endParaRPr lang="LID4096" sz="1100" b="0" cap="none" spc="0">
+            <a:ln w="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                <a:schemeClr val="dk1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1557,6 +1603,1496 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E10E3D9-057F-CDC1-F1EC-F5A563A78211}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4425950" y="3970337"/>
+          <a:ext cx="1320800" cy="282575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Signature</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2095500" cy="711200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Image 49">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5967935E-5935-4F5C-B69C-C025226134E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="19050" y="82550"/>
+          <a:ext cx="2095500" cy="711200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>334737</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="779688" cy="584200"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="51" name="Image 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6CBAD111-7DCB-42CE-B370-C679973BA552}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4906737" y="387350"/>
+          <a:ext cx="779688" cy="584200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4546600" cy="304800"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="52" name="ZoneTexte 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB127968-8C91-4A19-A997-803C33CF5D81}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="774700" y="831850"/>
+          <a:ext cx="4546600" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="2000" b="1"/>
+            <a:t>Reçu</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="2000" b="1" baseline="0"/>
+            <a:t> de paiement</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="2000" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>260350</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>272350</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="53" name="Rectangle 52">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{906DEBE6-6BC2-4314-B106-7CCD7F8EC72B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1022350" y="1562100"/>
+          <a:ext cx="774000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>69150</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="54" name="Rectangle 53">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9C89152-81AB-49B1-B435-7CCA8718F9B6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2343150" y="1562100"/>
+          <a:ext cx="774000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>520700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>532700</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="55" name="Rectangle 54">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5FC454B4-9EE1-49EE-913E-A84A32237698}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3568700" y="1562100"/>
+          <a:ext cx="774000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>280100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="56" name="Rectangle 55">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D47D32E3-1C8A-48D4-86E5-B8263CDE7BEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4852100" y="1562100"/>
+          <a:ext cx="774000" cy="317500"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="19050">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="LID4096" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>111125</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>120650</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>15875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="57" name="ZoneTexte 56">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A61BC76-E322-42A1-9488-C086045C642E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="171450" y="1584325"/>
+          <a:ext cx="711200" cy="273050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Produit :</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="58" name="ZoneTexte 57">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{04358429-76FC-42A3-A0F6-16EEEA77B7D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1028700" y="1235075"/>
+          <a:ext cx="781050" cy="273050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Voyage</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>50100</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>69150</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="59" name="ZoneTexte 58">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62872CE2-7C9C-4711-8D59-C34B2AFE0A4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2336100" y="1235075"/>
+          <a:ext cx="781050" cy="273050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Auto</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>513650</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>532700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="60" name="ZoneTexte 59">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C9851353-18A1-45D9-8CA5-1F5D7C45DEAD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3561650" y="1235075"/>
+          <a:ext cx="781050" cy="273050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Scolaire</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>273050</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>130175</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>34925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="61" name="ZoneTexte 60">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B04FAB47-8266-4485-900A-500DCEC1D5C0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4845050" y="1235075"/>
+          <a:ext cx="781050" cy="273050"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Accident</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>22225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>120650</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="62" name="ZoneTexte 61">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2698BD0B-F030-4A2E-B635-63373D9B08C4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31750" y="2232025"/>
+          <a:ext cx="628650" cy="282575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Date</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>7938</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>660400</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>106363</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="ZoneTexte 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E2DB4B32-97CF-488D-9766-CB67E40F9BE4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31750" y="2586038"/>
+          <a:ext cx="628650" cy="282575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Agence</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>482600</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>92076</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="64" name="ZoneTexte 63">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DA7F19A-1B05-4662-8914-C9CDEAC349F0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31750" y="2940051"/>
+          <a:ext cx="1212850" cy="282575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Nom</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0"/>
+            <a:t> du client</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>163514</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>146050</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>77789</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="65" name="ZoneTexte 64">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{981B5C9A-9A71-448A-88B4-F63613080FE9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31750" y="3294064"/>
+          <a:ext cx="876300" cy="282575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Période</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0"/>
+            <a:t> du</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>31750</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>149225</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>127000</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>63500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="66" name="ZoneTexte 65">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E20780FB-399F-4D11-AA42-6F4DC840F4D0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="31750" y="3648075"/>
+          <a:ext cx="857250" cy="282575"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1"/>
+            <a:t>Montant</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>755650</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="67" name="Connecteur droit 66">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{67717240-4D18-4DFA-8B72-2DB9306D26F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="755650" y="2762251"/>
+          <a:ext cx="4972050" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>726621</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>181428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="68" name="Connecteur droit 67">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E921B7D-7FBD-4ABC-9B71-03B06880CE62}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="726621" y="2391228"/>
+          <a:ext cx="5001079" cy="9072"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="69" name="Connecteur droit 68">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EA6C3B8D-12C5-4674-BC53-4A8FF7EFA2B5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="1016000" y="3124200"/>
+          <a:ext cx="4711700" cy="6351"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>177801</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="70" name="Connecteur droit 69">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{16D37CAC-CADB-48BC-8705-40FFF7150F64}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="838200" y="3486150"/>
+          <a:ext cx="4889500" cy="6351"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>44450</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="71" name="Connecteur droit 70">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C934654-EB93-4A10-951D-4B699BA9262B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="806450" y="3848100"/>
+          <a:ext cx="4921250" cy="19050"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="19050"/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>52</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="72" name="ZoneTexte 71">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53DF2C05-1D4B-493B-9721-0C2AC48C286E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3060700" y="3221037"/>
+          <a:ext cx="330200" cy="284163"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="fr-FR" sz="1100" b="1" baseline="0"/>
+            <a:t>au</a:t>
+          </a:r>
+          <a:endParaRPr lang="LID4096" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>615950</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>103187</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>412750</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>17462</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="73" name="ZoneTexte 72">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C31876E3-832F-4807-BE5E-205DD9C53B39}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1909,20 +3445,38 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B13:H21"/>
+  <dimension ref="A6:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21:H21"/>
+    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="13" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B13" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6" s="5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="3" t="str">
+        <f>IF(A6="AS1", "❌", "")</f>
+        <v>❌</v>
+      </c>
+      <c r="D10" s="4" t="str">
+        <f xml:space="preserve"> IF(A6="AS2", "❌", "")</f>
+        <v/>
+      </c>
+      <c r="F10" t="str">
+        <f xml:space="preserve"> IF(A6="AS3", "❌", "")</f>
+        <v/>
+      </c>
+      <c r="G10" s="3" t="str">
+        <f xml:space="preserve"> IF(A6="AS4", "❌", "")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
@@ -1931,9 +3485,89 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
+      <c r="H31" s="2"/>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B43" s="3" t="str">
+        <f>B10</f>
+        <v>❌</v>
+      </c>
+      <c r="D43" s="6" t="str">
+        <f>D10</f>
+        <v/>
+      </c>
+      <c r="F43" t="str">
+        <f>F10</f>
+        <v/>
+      </c>
+      <c r="G43" s="3" t="str">
+        <f>G10</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <f>B13</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <f>B15</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C50">
+        <f>C17</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C52">
+        <f>C19</f>
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <f>F19</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54" s="1"/>
+      <c r="C54" s="1">
+        <f>C21</f>
+        <v>0</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+      <c r="F54" s="1"/>
+      <c r="G54" s="1"/>
+      <c r="H54" s="1"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.47244094488188981" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" scale="99" orientation="portrait"/>
-  <drawing r:id="rId1"/>
+  <conditionalFormatting sqref="A6">
+    <cfRule type="iconSet" priority="1">
+      <iconSet iconSet="3Symbols2">
+        <cfvo type="percent" val="0"/>
+        <cfvo type="percent" val="33"/>
+        <cfvo type="percent" val="67"/>
+      </iconSet>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="1" right="1" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" scale="83" orientation="portrait" r:id="rId1"/>
+  <colBreaks count="1" manualBreakCount="1">
+    <brk id="7" max="1048575" man="1"/>
+  </colBreaks>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Modification des élément du fichier excel
</commit_message>
<xml_diff>
--- a/PrintExcelToPdf/Templates/template_sunu.xlsx
+++ b/PrintExcelToPdf/Templates/template_sunu.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gedeo\source\repos\PrintExcelToPdf\PrintExcelToPdf\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660A3D7B-BFA2-4687-838D-7801C0FD70B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E235681-072B-463B-990B-8A17BFFF47D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{BDB7740D-B914-44FE-88FD-0981D9AB0366}"/>
   </bookViews>
@@ -46,7 +46,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -64,6 +64,22 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,20 +115,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Milliers" xfId="1" builtinId="3"/>
@@ -3447,32 +3464,32 @@
   </sheetPr>
   <dimension ref="A6:H54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G43" sqref="G43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="B10" s="3" t="str">
-        <f>IF(A6="AS1", "❌", "")</f>
-        <v>❌</v>
+    <row r="10" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="B10" s="5" t="str">
+        <f>IF(A6="AS1", "X", "")</f>
+        <v>X</v>
       </c>
-      <c r="D10" s="4" t="str">
-        <f xml:space="preserve"> IF(A6="AS2", "❌", "")</f>
+      <c r="D10" s="5" t="str">
+        <f xml:space="preserve"> IF(A6="AS2", "X", "")</f>
         <v/>
       </c>
-      <c r="F10" t="str">
-        <f xml:space="preserve"> IF(A6="AS3", "❌", "")</f>
+      <c r="F10" s="5" t="str">
+        <f xml:space="preserve"> IF(A6="AS3", "X", "")</f>
         <v/>
       </c>
-      <c r="G10" s="3" t="str">
-        <f xml:space="preserve"> IF(A6="AS4", "❌", "")</f>
+      <c r="G10" s="5" t="str">
+        <f xml:space="preserve"> IF(A6="AS4", "X", "")</f>
         <v/>
       </c>
     </row>
@@ -3496,19 +3513,19 @@
       <c r="H31" s="2"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="B43" s="3" t="str">
+      <c r="B43" s="4" t="str">
         <f>B10</f>
-        <v>❌</v>
+        <v>X</v>
       </c>
       <c r="D43" s="6" t="str">
         <f>D10</f>
         <v/>
       </c>
-      <c r="F43" t="str">
+      <c r="F43" s="7" t="str">
         <f>F10</f>
         <v/>
       </c>
-      <c r="G43" s="3" t="str">
+      <c r="G43" s="4" t="str">
         <f>G10</f>
         <v/>
       </c>

</xml_diff>